<commit_message>
upd doc structure and organisational stuff
</commit_message>
<xml_diff>
--- a/documentation/PPL_Gitcon_GruS.xlsx
+++ b/documentation/PPL_Gitcon_GruS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smon\source\MTAP-MIDI-Guitar-Converter\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A765AD-EB44-499B-BD12-5D0429668872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD911F76-495E-4D72-87AA-C6604E43F334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Dauer</t>
   </si>
@@ -225,10 +225,13 @@
     <t>Aufsetzung der Treiber und Software</t>
   </si>
   <si>
-    <t>Bestellung des Mainboards</t>
-  </si>
-  <si>
     <t>Planung des Prototypen</t>
+  </si>
+  <si>
+    <t>PCB Spezifikationen und Design</t>
+  </si>
+  <si>
+    <t>Review und Bestellung des Mainboards</t>
   </si>
 </sst>
 </file>
@@ -1055,6 +1058,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1076,7 +1080,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1418,7 +1421,7 @@
   <dimension ref="A1:AX34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1446,48 +1449,48 @@
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
       <c r="M1" s="32"/>
-      <c r="N1" s="76" t="s">
+      <c r="N1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="76" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="76" t="s">
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="77"/>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="79"/>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -1505,66 +1508,66 @@
       <c r="I2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74" t="s">
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="74" t="s">
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="74" t="s">
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="74" t="s">
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
-      <c r="AC2" s="74"/>
-      <c r="AD2" s="74" t="s">
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="74"/>
-      <c r="AF2" s="74"/>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="74" t="s">
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="74"/>
-      <c r="AK2" s="74"/>
-      <c r="AL2" s="74" t="s">
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="74"/>
-      <c r="AP2" s="74" t="s">
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="74"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="74" t="s">
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="AU2" s="74"/>
-      <c r="AV2" s="74"/>
-      <c r="AW2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
+      <c r="AW2" s="76"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
@@ -1909,8 +1912,8 @@
         <v>7</v>
       </c>
       <c r="B9" s="59"/>
-      <c r="C9" s="79" t="s">
-        <v>54</v>
+      <c r="C9" s="72" t="s">
+        <v>53</v>
       </c>
       <c r="D9" s="62"/>
       <c r="E9" s="62"/>
@@ -1974,7 +1977,9 @@
       <c r="F10" s="62"/>
       <c r="G10" s="19"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="66"/>
+      <c r="I10" s="66">
+        <v>10</v>
+      </c>
       <c r="J10" s="36"/>
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
@@ -2021,13 +2026,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="59"/>
-      <c r="C11" s="62"/>
+      <c r="C11" s="62" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="62"/>
       <c r="E11" s="62"/>
       <c r="F11" s="62"/>
       <c r="G11" s="19"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="66"/>
+      <c r="I11" s="66">
+        <v>30</v>
+      </c>
       <c r="J11" s="36"/>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
@@ -2083,7 +2092,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="23"/>
       <c r="I12" s="66">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J12" s="36"/>
       <c r="K12" s="38"/>
@@ -2311,7 +2320,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="23"/>
       <c r="I16" s="66">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J16" s="36"/>
       <c r="K16" s="38"/>
@@ -2417,7 +2426,7 @@
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="62" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" s="62"/>
       <c r="E18" s="62"/>
@@ -2828,25 +2837,25 @@
       <c r="O25" s="38"/>
       <c r="P25" s="38"/>
       <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-      <c r="AF25" s="38"/>
-      <c r="AG25" s="38"/>
-      <c r="AH25" s="38"/>
-      <c r="AI25" s="38"/>
-      <c r="AJ25" s="38"/>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="52"/>
+      <c r="V25" s="52"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52"/>
+      <c r="Y25" s="52"/>
+      <c r="Z25" s="52"/>
+      <c r="AA25" s="52"/>
+      <c r="AB25" s="52"/>
+      <c r="AC25" s="52"/>
+      <c r="AD25" s="52"/>
+      <c r="AE25" s="52"/>
+      <c r="AF25" s="52"/>
+      <c r="AG25" s="52"/>
+      <c r="AH25" s="52"/>
+      <c r="AI25" s="52"/>
+      <c r="AJ25" s="52"/>
       <c r="AK25" s="37"/>
       <c r="AL25" s="37"/>
       <c r="AM25" s="70"/>
@@ -2982,7 +2991,7 @@
       </c>
       <c r="I28" s="68">
         <f>SUM(I3:I27)</f>
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="AW28" s="5"/>
     </row>
@@ -3159,12 +3168,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3300,15 +3306,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADAFA77-C44E-4145-B33E-4C0DA35AE6B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81E45984-FD63-4A1D-8AA0-E48F278C1B4D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc157ffa-89df-417c-a5af-b14496f38a84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3332,17 +3349,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81E45984-FD63-4A1D-8AA0-E48F278C1B4D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADAFA77-C44E-4145-B33E-4C0DA35AE6B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc157ffa-89df-417c-a5af-b14496f38a84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>